<commit_message>
leçon 2 et 3
</commit_message>
<xml_diff>
--- a/horaire.xlsx
+++ b/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/projets/developpementweb3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF8887D-BA65-0246-A9F5-F8927B7C2990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8F23A8-3EE1-C847-A76A-1D8A2529B64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8880" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -140,12 +140,6 @@
     <t>Exercice</t>
   </si>
   <si>
-    <t>npm</t>
-  </si>
-  <si>
-    <t>TypeScript - La suite</t>
-  </si>
-  <si>
     <t>Express</t>
   </si>
   <si>
@@ -195,6 +189,18 @@
   </si>
   <si>
     <t>[Introduction à Node.js](introduction_nodejs.md) &lt;br/&gt; [Introduction à TypeScript](introduction_typescript.md) &lt;br/&gt; [Node.js - Serveur Web](nodejs_serveur_web.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 2 - lodash](exercice2_lodash.md)</t>
+  </si>
+  <si>
+    <t>[npm](npm.md)</t>
+  </si>
+  <si>
+    <t>[TypeScript 2](typescript_2.md)&lt;br/&gt;[Introduction Express](introduction_express.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 3 - Express](exercice3_express.md)</t>
   </si>
 </sst>
 </file>
@@ -576,7 +582,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,10 +613,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -621,7 +627,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -632,7 +641,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -643,7 +655,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -654,7 +666,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -665,7 +677,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -676,7 +688,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -687,7 +699,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -698,7 +710,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -709,7 +721,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -720,7 +732,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -731,7 +743,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -742,7 +754,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -753,7 +765,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -764,7 +776,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -775,7 +787,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -786,7 +798,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -797,7 +809,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -808,7 +820,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -819,7 +831,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -830,7 +842,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -841,7 +853,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -852,7 +864,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -863,7 +875,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -874,7 +886,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -885,7 +897,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -896,7 +908,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -907,7 +919,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -918,7 +930,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -929,7 +941,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lecon 4 et début 5
</commit_message>
<xml_diff>
--- a/horaire.xlsx
+++ b/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/projets/developpementweb3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8F23A8-3EE1-C847-A76A-1D8A2529B64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40E47EB-196B-FB44-9763-087DF77AA4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8880" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -140,12 +140,6 @@
     <t>Exercice</t>
   </si>
   <si>
-    <t>Express</t>
-  </si>
-  <si>
-    <t>MongoDB</t>
-  </si>
-  <si>
     <t>Mongoose</t>
   </si>
   <si>
@@ -201,6 +195,18 @@
   </si>
   <si>
     <t>[Exercice 3 - Express](exercice3_express.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 4 - Express avec modèle](exercice4_express_avec_modele.md)</t>
+  </si>
+  <si>
+    <t>[Express - Générateur](generateur_express.md)</t>
+  </si>
+  <si>
+    <t>[JavaScript asynchrone](javascript_async.md) &lt;br/&gt; [MongoDB](mongodb.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 5 - MongoDB](exercice5_mongodb.md)</t>
   </si>
 </sst>
 </file>
@@ -582,7 +588,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,10 +619,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -627,10 +633,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -641,10 +647,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -655,7 +661,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -666,7 +675,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -677,7 +689,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -688,7 +700,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -699,7 +711,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -710,7 +722,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -721,7 +733,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -732,7 +744,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -743,7 +755,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -754,7 +766,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -765,7 +777,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -776,7 +788,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -787,7 +799,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -798,7 +810,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -809,7 +821,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -820,7 +832,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -831,7 +843,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -842,7 +854,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -853,7 +865,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -864,7 +876,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -875,7 +887,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -886,7 +898,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -897,7 +909,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -908,7 +920,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -919,7 +931,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -930,7 +942,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -941,7 +953,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
leçons 6 et 7
</commit_message>
<xml_diff>
--- a/horaire.xlsx
+++ b/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/projets/developpementweb3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5016826E-A667-4D43-B507-DACD5917EDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A14B31-4532-E540-A99A-4EAFDEF849DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8880" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Exercice</t>
   </si>
   <si>
-    <t>Mongoose</t>
-  </si>
-  <si>
     <t>Évaluation formative</t>
   </si>
   <si>
@@ -207,6 +204,18 @@
   </si>
   <si>
     <t>[Exercice 5 - MongoDB](exercice5_mongodb.md)</t>
+  </si>
+  <si>
+    <t>[Mongoose](introduction_mongoose.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 6 - Mongoose](exercice6_mongoose.md)</t>
+  </si>
+  <si>
+    <t>[Mongoose - la suite](mongoose2.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 7 - Mongoose](exercice7_mongoose.md)</t>
   </si>
 </sst>
 </file>
@@ -588,7 +597,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -619,10 +628,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,10 +642,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -647,10 +656,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
         <v>51</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -661,10 +670,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -675,10 +684,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
         <v>55</v>
-      </c>
-      <c r="D6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -689,7 +698,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -700,7 +712,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -711,7 +726,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -722,7 +737,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -733,7 +748,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -744,7 +759,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -755,7 +770,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -766,7 +781,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -777,7 +792,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -788,7 +803,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -799,7 +814,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -810,7 +825,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -821,7 +836,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -832,7 +847,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -843,7 +858,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -854,7 +869,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -865,7 +880,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -876,7 +891,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -887,7 +902,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -898,7 +913,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -909,7 +924,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -920,7 +935,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -931,7 +946,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -942,7 +957,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -953,7 +968,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>